<commit_message>
Finished group DataFrame, started scoring groups
</commit_message>
<xml_diff>
--- a/groups.xlsx
+++ b/groups.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +524,11 @@
           <t>Esubject</t>
         </is>
       </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>MatchingInterests</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -616,6 +621,11 @@
           <t>['Physics', 'Math']</t>
         </is>
       </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Handicrafts,History,Technology,Physics,</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -708,6 +718,11 @@
           <t>['English', 'Social Studies']</t>
         </is>
       </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Philosophy,English,Social Studies,</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -800,6 +815,11 @@
           <t>['Physics', 'English']</t>
         </is>
       </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Gardening,Physics,</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -892,6 +912,11 @@
           <t>['Physics', 'Math']</t>
         </is>
       </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Gardening,Emotional Regulation,Technology,Physics,</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -982,6 +1007,11 @@
       <c r="R6" t="inlineStr">
         <is>
           <t>['Chemistry']</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Cooking,Baking,Apps,Chemistry,</t>
         </is>
       </c>
     </row>

</xml_diff>